<commit_message>
Update BaoCaoSanLuongToanCongTy and BangCap_GiayChungNhan
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/DK/DailyDepartment/templateBaoCaoTheoPhanXuong.xlsx
+++ b/QUANGHANH2/excel/DK/DailyDepartment/templateBaoCaoTheoPhanXuong.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quoct\Documents\GitHub\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\DK\DailyDepartment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SAP-LAB-PROJECTS\Dự án\2019\Dự Án Than Quang Hanh\FROM GIT MASTER (San Xuat Cu)\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\DK\DailyDepartment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E4FE4D-258D-440E-90F7-2E54829CB21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{06331CE9-B319-4A64-BAC3-8E1F34E2502B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15996"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -87,13 +86,16 @@
     <t>GHI CHÚ</t>
   </si>
   <si>
-    <t>KHĐC                       (Tăng 3-5%)</t>
+    <t>KHBĐ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHĐC                      </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -167,6 +169,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,64 +486,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0453357E-5159-4AA2-B798-E49FECBC0A71}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
-    <col min="4" max="11" width="9.140625" style="3"/>
-    <col min="12" max="12" width="16" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="7.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="3" customWidth="1"/>
+    <col min="4" max="10" width="9.109375" style="3"/>
+    <col min="11" max="11" width="11.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+    <row r="2" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,29 +571,32 @@
       <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="2"/>
+      <c r="Q2" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>